<commit_message>
CIERRE 13 FEB 2023
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CREDITOS     ZAVALETA  ENERO 2023.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CREDITOS     ZAVALETA  ENERO 2023.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t xml:space="preserve">ABASTO 4 CARNES    Z A V A L E T A </t>
   </si>
@@ -154,7 +154,13 @@
     <t>ALBICIA</t>
   </si>
   <si>
-    <t>15-Ene-23--18-Ene-23--</t>
+    <t>15-Ene-23--18-Ene-23--22-ENE-23</t>
+  </si>
+  <si>
+    <t>23-Ene-23--24-Ene-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HERRADURA </t>
   </si>
 </sst>
 </file>
@@ -747,7 +753,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -909,7 +915,6 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -990,42 +995,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1046,6 +1021,33 @@
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="15" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1493,7 +1495,10 @@
   <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1503,32 +1508,32 @@
     <col min="3" max="3" width="9.85546875" style="72" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="34.28515625" style="73" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" style="74" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="144" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="133" customWidth="1"/>
     <col min="7" max="7" width="18" style="75" customWidth="1"/>
     <col min="8" max="8" width="14.140625" customWidth="1"/>
     <col min="9" max="9" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="126" t="s">
+      <c r="B1" s="134" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="128"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
+      <c r="E1" s="135"/>
+      <c r="F1" s="135"/>
+      <c r="G1" s="136"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="129" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="129"/>
-      <c r="D2" s="129"/>
-      <c r="E2" s="129"/>
-      <c r="F2" s="129"/>
+      <c r="B2" s="137" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="137"/>
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
@@ -1566,13 +1571,13 @@
         <v>608</v>
       </c>
       <c r="C4" s="16"/>
-      <c r="D4" s="125" t="s">
+      <c r="D4" s="124" t="s">
         <v>22</v>
       </c>
       <c r="E4" s="18">
         <v>0</v>
       </c>
-      <c r="F4" s="135"/>
+      <c r="F4" s="125"/>
       <c r="G4" s="76"/>
       <c r="H4" s="19">
         <f t="shared" ref="H4:H47" si="0">E4-G4</f>
@@ -1594,11 +1599,15 @@
       <c r="E5" s="20">
         <v>22440</v>
       </c>
-      <c r="F5" s="136"/>
-      <c r="G5" s="21"/>
+      <c r="F5" s="126">
+        <v>44952</v>
+      </c>
+      <c r="G5" s="21">
+        <v>22440</v>
+      </c>
       <c r="H5" s="19">
         <f t="shared" si="0"/>
-        <v>22440</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1615,11 +1624,15 @@
       <c r="E6" s="20">
         <v>3668</v>
       </c>
-      <c r="F6" s="136"/>
-      <c r="G6" s="21"/>
+      <c r="F6" s="126">
+        <v>44952</v>
+      </c>
+      <c r="G6" s="21">
+        <v>3668</v>
+      </c>
       <c r="H6" s="19">
         <f t="shared" si="0"/>
-        <v>3668</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1636,7 +1649,7 @@
       <c r="E7" s="20">
         <v>681</v>
       </c>
-      <c r="F7" s="136">
+      <c r="F7" s="126">
         <v>44944</v>
       </c>
       <c r="G7" s="21">
@@ -1659,13 +1672,17 @@
         <v>23</v>
       </c>
       <c r="E8" s="20">
-        <v>2808</v>
-      </c>
-      <c r="F8" s="137"/>
-      <c r="G8" s="77"/>
+        <v>28080</v>
+      </c>
+      <c r="F8" s="126">
+        <v>44952</v>
+      </c>
+      <c r="G8" s="21">
+        <v>28080</v>
+      </c>
       <c r="H8" s="25">
         <f t="shared" si="0"/>
-        <v>2808</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
@@ -1676,13 +1693,13 @@
         <v>613</v>
       </c>
       <c r="C9" s="26"/>
-      <c r="D9" s="124" t="s">
+      <c r="D9" s="123" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="20">
         <v>6045</v>
       </c>
-      <c r="F9" s="136">
+      <c r="F9" s="126">
         <v>44939</v>
       </c>
       <c r="G9" s="21">
@@ -1707,11 +1724,15 @@
       <c r="E10" s="20">
         <v>10290</v>
       </c>
-      <c r="F10" s="137"/>
-      <c r="G10" s="77"/>
+      <c r="F10" s="126">
+        <v>44952</v>
+      </c>
+      <c r="G10" s="21">
+        <v>10290</v>
+      </c>
       <c r="H10" s="19">
         <f t="shared" si="0"/>
-        <v>10290</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1728,7 +1749,7 @@
       <c r="E11" s="20">
         <v>2897</v>
       </c>
-      <c r="F11" s="136">
+      <c r="F11" s="126">
         <v>44939</v>
       </c>
       <c r="G11" s="21">
@@ -1739,7 +1760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
         <v>44940</v>
       </c>
@@ -1753,16 +1774,16 @@
       <c r="E12" s="20">
         <v>28065</v>
       </c>
-      <c r="F12" s="136" t="s">
+      <c r="F12" s="126" t="s">
         <v>29</v>
       </c>
       <c r="G12" s="21">
-        <f>5000+10800</f>
-        <v>15800</v>
+        <f>5080+10800+12185</f>
+        <v>28065</v>
       </c>
       <c r="H12" s="19">
         <f t="shared" si="0"/>
-        <v>12265</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1779,11 +1800,15 @@
       <c r="E13" s="20">
         <v>5586</v>
       </c>
-      <c r="F13" s="137"/>
-      <c r="G13" s="77"/>
+      <c r="F13" s="126">
+        <v>44952</v>
+      </c>
+      <c r="G13" s="21">
+        <v>5586</v>
+      </c>
       <c r="H13" s="19">
         <f t="shared" si="0"/>
-        <v>5586</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1800,11 +1825,15 @@
       <c r="E14" s="20">
         <v>4950</v>
       </c>
-      <c r="F14" s="136"/>
-      <c r="G14" s="21"/>
+      <c r="F14" s="126">
+        <v>44952</v>
+      </c>
+      <c r="G14" s="21">
+        <v>4950</v>
+      </c>
       <c r="H14" s="19">
         <f t="shared" si="0"/>
-        <v>4950</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1821,7 +1850,7 @@
       <c r="E15" s="20">
         <v>250</v>
       </c>
-      <c r="F15" s="136"/>
+      <c r="F15" s="126"/>
       <c r="G15" s="21"/>
       <c r="H15" s="19">
         <f t="shared" si="0"/>
@@ -1842,11 +1871,15 @@
       <c r="E16" s="20">
         <v>1284</v>
       </c>
-      <c r="F16" s="137"/>
-      <c r="G16" s="77"/>
+      <c r="F16" s="126">
+        <v>44951</v>
+      </c>
+      <c r="G16" s="21">
+        <v>1284</v>
+      </c>
       <c r="H16" s="19">
         <f t="shared" si="0"/>
-        <v>1284</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1863,11 +1896,15 @@
       <c r="E17" s="20">
         <v>7591</v>
       </c>
-      <c r="F17" s="136"/>
-      <c r="G17" s="21"/>
+      <c r="F17" s="126">
+        <v>44947</v>
+      </c>
+      <c r="G17" s="21">
+        <v>7591</v>
+      </c>
       <c r="H17" s="19">
         <f t="shared" si="0"/>
-        <v>7591</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1884,116 +1921,179 @@
       <c r="E18" s="20">
         <v>13942</v>
       </c>
-      <c r="F18" s="136"/>
-      <c r="G18" s="21"/>
+      <c r="F18" s="126">
+        <v>44952</v>
+      </c>
+      <c r="G18" s="21">
+        <v>13942</v>
+      </c>
       <c r="H18" s="19">
         <f t="shared" si="0"/>
-        <v>13942</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
+      <c r="A19" s="14">
+        <v>44946</v>
+      </c>
       <c r="B19" s="15">
         <v>623</v>
       </c>
       <c r="C19" s="29"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="137"/>
-      <c r="G19" s="77"/>
+      <c r="D19" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="20">
+        <v>9350</v>
+      </c>
+      <c r="F19" s="126">
+        <v>44942</v>
+      </c>
+      <c r="G19" s="21">
+        <v>9350</v>
+      </c>
       <c r="H19" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
+      <c r="A20" s="14">
+        <v>44947</v>
+      </c>
       <c r="B20" s="15">
         <v>624</v>
       </c>
       <c r="C20" s="28"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="137"/>
-      <c r="G20" s="77"/>
+      <c r="D20" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="20">
+        <v>26352</v>
+      </c>
+      <c r="F20" s="126">
+        <v>44952</v>
+      </c>
+      <c r="G20" s="21">
+        <v>26352</v>
+      </c>
       <c r="H20" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
+    <row r="21" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="14">
+        <v>44948</v>
+      </c>
       <c r="B21" s="15">
         <v>625</v>
       </c>
       <c r="C21" s="28"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="136"/>
-      <c r="G21" s="21"/>
+      <c r="D21" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="20">
+        <v>21187</v>
+      </c>
+      <c r="F21" s="126" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="21">
+        <f>6100+9800+4000+1287</f>
+        <v>21187</v>
+      </c>
       <c r="H21" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
+      <c r="A22" s="14">
+        <v>44951</v>
+      </c>
       <c r="B22" s="15">
         <v>626</v>
       </c>
       <c r="C22" s="28"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="137"/>
-      <c r="G22" s="77"/>
+      <c r="D22" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="20">
+        <v>1174</v>
+      </c>
+      <c r="F22" s="126"/>
+      <c r="G22" s="21"/>
       <c r="H22" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
+      <c r="A23" s="14">
+        <v>44951</v>
+      </c>
       <c r="B23" s="15">
         <v>627</v>
       </c>
       <c r="C23" s="28"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="136"/>
-      <c r="G23" s="21"/>
+      <c r="D23" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="20">
+        <v>2842</v>
+      </c>
+      <c r="F23" s="126">
+        <v>44951</v>
+      </c>
+      <c r="G23" s="21">
+        <v>2842</v>
+      </c>
       <c r="H23" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
+      <c r="A24" s="14">
+        <v>44951</v>
+      </c>
       <c r="B24" s="15">
         <v>628</v>
       </c>
       <c r="C24" s="28"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="136"/>
+      <c r="D24" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="20">
+        <v>9540</v>
+      </c>
+      <c r="F24" s="126"/>
       <c r="G24" s="21"/>
       <c r="H24" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9540</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
+      <c r="A25" s="22">
+        <v>44952</v>
+      </c>
       <c r="B25" s="15">
         <v>629</v>
       </c>
       <c r="C25" s="28"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="137"/>
-      <c r="G25" s="77"/>
+      <c r="D25" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="20">
+        <v>90643</v>
+      </c>
+      <c r="F25" s="126"/>
+      <c r="G25" s="21"/>
       <c r="H25" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>90643</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2004,7 +2104,7 @@
       <c r="C26" s="28"/>
       <c r="D26" s="17"/>
       <c r="E26" s="20"/>
-      <c r="F26" s="136"/>
+      <c r="F26" s="126"/>
       <c r="G26" s="21"/>
       <c r="H26" s="19">
         <f t="shared" si="0"/>
@@ -2019,7 +2119,7 @@
       <c r="C27" s="28"/>
       <c r="D27" s="17"/>
       <c r="E27" s="20"/>
-      <c r="F27" s="136"/>
+      <c r="F27" s="126"/>
       <c r="G27" s="21"/>
       <c r="H27" s="19">
         <f t="shared" si="0"/>
@@ -2034,7 +2134,7 @@
       <c r="C28" s="28"/>
       <c r="D28" s="27"/>
       <c r="E28" s="20"/>
-      <c r="F28" s="136"/>
+      <c r="F28" s="126"/>
       <c r="G28" s="21"/>
       <c r="H28" s="19">
         <f t="shared" si="0"/>
@@ -2049,8 +2149,8 @@
       <c r="C29" s="28"/>
       <c r="D29" s="17"/>
       <c r="E29" s="20"/>
-      <c r="F29" s="137"/>
-      <c r="G29" s="77"/>
+      <c r="F29" s="126"/>
+      <c r="G29" s="21"/>
       <c r="H29" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2064,8 +2164,8 @@
       <c r="C30" s="28"/>
       <c r="D30" s="17"/>
       <c r="E30" s="20"/>
-      <c r="F30" s="137"/>
-      <c r="G30" s="77"/>
+      <c r="F30" s="126"/>
+      <c r="G30" s="21"/>
       <c r="H30" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2079,8 +2179,8 @@
       <c r="C31" s="28"/>
       <c r="D31" s="17"/>
       <c r="E31" s="20"/>
-      <c r="F31" s="137"/>
-      <c r="G31" s="77"/>
+      <c r="F31" s="126"/>
+      <c r="G31" s="21"/>
       <c r="H31" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2094,8 +2194,8 @@
       <c r="C32" s="28"/>
       <c r="D32" s="17"/>
       <c r="E32" s="20"/>
-      <c r="F32" s="137"/>
-      <c r="G32" s="77"/>
+      <c r="F32" s="126"/>
+      <c r="G32" s="21"/>
       <c r="H32" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2109,7 +2209,7 @@
       <c r="C33" s="28"/>
       <c r="D33" s="17"/>
       <c r="E33" s="20"/>
-      <c r="F33" s="136"/>
+      <c r="F33" s="126"/>
       <c r="G33" s="21"/>
       <c r="H33" s="19">
         <f t="shared" si="0"/>
@@ -2124,8 +2224,8 @@
       <c r="C34" s="28"/>
       <c r="D34" s="17"/>
       <c r="E34" s="20"/>
-      <c r="F34" s="137"/>
-      <c r="G34" s="77"/>
+      <c r="F34" s="126"/>
+      <c r="G34" s="21"/>
       <c r="H34" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2139,8 +2239,8 @@
       <c r="C35" s="28"/>
       <c r="D35" s="17"/>
       <c r="E35" s="20"/>
-      <c r="F35" s="137"/>
-      <c r="G35" s="77"/>
+      <c r="F35" s="126"/>
+      <c r="G35" s="21"/>
       <c r="H35" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2154,8 +2254,8 @@
       <c r="C36" s="28"/>
       <c r="D36" s="17"/>
       <c r="E36" s="20"/>
-      <c r="F36" s="137"/>
-      <c r="G36" s="77"/>
+      <c r="F36" s="126"/>
+      <c r="G36" s="21"/>
       <c r="H36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2169,7 +2269,7 @@
       <c r="C37" s="28"/>
       <c r="D37" s="17"/>
       <c r="E37" s="20"/>
-      <c r="F37" s="136"/>
+      <c r="F37" s="126"/>
       <c r="G37" s="21"/>
       <c r="H37" s="19">
         <f t="shared" si="0"/>
@@ -2184,8 +2284,8 @@
       <c r="C38" s="28"/>
       <c r="D38" s="17"/>
       <c r="E38" s="20"/>
-      <c r="F38" s="137"/>
-      <c r="G38" s="77"/>
+      <c r="F38" s="126"/>
+      <c r="G38" s="21"/>
       <c r="H38" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2199,7 +2299,7 @@
       <c r="C39" s="28"/>
       <c r="D39" s="17"/>
       <c r="E39" s="20"/>
-      <c r="F39" s="136"/>
+      <c r="F39" s="126"/>
       <c r="G39" s="21"/>
       <c r="H39" s="19">
         <f t="shared" si="0"/>
@@ -2214,7 +2314,7 @@
       <c r="C40" s="28"/>
       <c r="D40" s="17"/>
       <c r="E40" s="20"/>
-      <c r="F40" s="136"/>
+      <c r="F40" s="126"/>
       <c r="G40" s="21"/>
       <c r="H40" s="19">
         <f t="shared" si="0"/>
@@ -2229,8 +2329,8 @@
       <c r="C41" s="28"/>
       <c r="D41" s="17"/>
       <c r="E41" s="20"/>
-      <c r="F41" s="137"/>
-      <c r="G41" s="77"/>
+      <c r="F41" s="126"/>
+      <c r="G41" s="21"/>
       <c r="H41" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2244,8 +2344,8 @@
       <c r="C42" s="28"/>
       <c r="D42" s="17"/>
       <c r="E42" s="20"/>
-      <c r="F42" s="137"/>
-      <c r="G42" s="77"/>
+      <c r="F42" s="126"/>
+      <c r="G42" s="21"/>
       <c r="H42" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2259,8 +2359,8 @@
       <c r="C43" s="28"/>
       <c r="D43" s="17"/>
       <c r="E43" s="20"/>
-      <c r="F43" s="137"/>
-      <c r="G43" s="77"/>
+      <c r="F43" s="126"/>
+      <c r="G43" s="21"/>
       <c r="H43" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2274,8 +2374,8 @@
       <c r="C44" s="28"/>
       <c r="D44" s="17"/>
       <c r="E44" s="20"/>
-      <c r="F44" s="137"/>
-      <c r="G44" s="77"/>
+      <c r="F44" s="126"/>
+      <c r="G44" s="21"/>
       <c r="H44" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2289,7 +2389,7 @@
       <c r="C45" s="28"/>
       <c r="D45" s="17"/>
       <c r="E45" s="20"/>
-      <c r="F45" s="136"/>
+      <c r="F45" s="126"/>
       <c r="G45" s="21"/>
       <c r="H45" s="19">
         <f t="shared" si="0"/>
@@ -2304,7 +2404,7 @@
       <c r="C46" s="28"/>
       <c r="D46" s="17"/>
       <c r="E46" s="20"/>
-      <c r="F46" s="136"/>
+      <c r="F46" s="126"/>
       <c r="G46" s="21"/>
       <c r="H46" s="19">
         <f t="shared" si="0"/>
@@ -2319,7 +2419,7 @@
       <c r="E47" s="36">
         <v>0</v>
       </c>
-      <c r="F47" s="138"/>
+      <c r="F47" s="127"/>
       <c r="G47" s="37"/>
       <c r="H47" s="19">
         <f t="shared" si="0"/>
@@ -2333,16 +2433,16 @@
       <c r="D48" s="40"/>
       <c r="E48" s="41">
         <f>SUM(E4:E47)</f>
-        <v>110497</v>
-      </c>
-      <c r="F48" s="139"/>
+        <v>296857</v>
+      </c>
+      <c r="F48" s="128"/>
       <c r="G48" s="41">
         <f>SUM(G4:G47)</f>
-        <v>25423</v>
+        <v>195250</v>
       </c>
       <c r="H48" s="42">
         <f>SUM(H23:H47)</f>
-        <v>0</v>
+        <v>100183</v>
       </c>
       <c r="I48" s="2"/>
     </row>
@@ -2351,7 +2451,7 @@
       <c r="C49" s="39"/>
       <c r="D49" s="40"/>
       <c r="E49" s="43"/>
-      <c r="F49" s="140"/>
+      <c r="F49" s="129"/>
       <c r="G49" s="44"/>
       <c r="H49" s="45"/>
       <c r="I49" s="2"/>
@@ -2363,7 +2463,7 @@
       <c r="E50" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="F50" s="140"/>
+      <c r="F50" s="129"/>
       <c r="G50" s="47" t="s">
         <v>9</v>
       </c>
@@ -2375,7 +2475,7 @@
       <c r="C51" s="39"/>
       <c r="D51" s="40"/>
       <c r="E51" s="46"/>
-      <c r="F51" s="140"/>
+      <c r="F51" s="129"/>
       <c r="G51" s="47"/>
       <c r="H51" s="45"/>
       <c r="I51" s="2"/>
@@ -2384,12 +2484,12 @@
       <c r="B52" s="38"/>
       <c r="C52" s="39"/>
       <c r="D52" s="40"/>
-      <c r="E52" s="130">
+      <c r="E52" s="138">
         <f>E48-G48</f>
-        <v>85074</v>
-      </c>
-      <c r="F52" s="131"/>
-      <c r="G52" s="132"/>
+        <v>101607</v>
+      </c>
+      <c r="F52" s="139"/>
+      <c r="G52" s="140"/>
       <c r="I52" s="2"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -2397,7 +2497,7 @@
       <c r="C53" s="39"/>
       <c r="D53" s="40"/>
       <c r="E53" s="43"/>
-      <c r="F53" s="140"/>
+      <c r="F53" s="129"/>
       <c r="G53" s="44"/>
       <c r="I53" s="2"/>
     </row>
@@ -2405,11 +2505,11 @@
       <c r="B54" s="38"/>
       <c r="C54" s="39"/>
       <c r="D54" s="40"/>
-      <c r="E54" s="133" t="s">
+      <c r="E54" s="141" t="s">
         <v>10</v>
       </c>
-      <c r="F54" s="133"/>
-      <c r="G54" s="133"/>
+      <c r="F54" s="141"/>
+      <c r="G54" s="141"/>
       <c r="I54" s="2"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -2417,7 +2517,7 @@
       <c r="C55" s="49"/>
       <c r="D55" s="50"/>
       <c r="E55" s="51"/>
-      <c r="F55" s="141"/>
+      <c r="F55" s="130"/>
       <c r="G55" s="52"/>
       <c r="I55" s="2"/>
     </row>
@@ -2438,7 +2538,7 @@
       <c r="C57" s="62"/>
       <c r="D57" s="63"/>
       <c r="E57" s="64"/>
-      <c r="F57" s="142"/>
+      <c r="F57" s="131"/>
       <c r="G57" s="65"/>
       <c r="H57" s="59"/>
       <c r="I57" s="2"/>
@@ -2449,7 +2549,7 @@
       <c r="C58" s="62"/>
       <c r="D58" s="63"/>
       <c r="E58" s="64"/>
-      <c r="F58" s="142"/>
+      <c r="F58" s="131"/>
       <c r="G58" s="65"/>
       <c r="H58" s="59"/>
       <c r="I58" s="2"/>
@@ -2460,7 +2560,7 @@
       <c r="C59" s="62"/>
       <c r="D59" s="63"/>
       <c r="E59" s="64"/>
-      <c r="F59" s="142"/>
+      <c r="F59" s="131"/>
       <c r="G59" s="65"/>
       <c r="H59" s="59"/>
       <c r="I59" s="2"/>
@@ -2471,7 +2571,7 @@
       <c r="C60" s="62"/>
       <c r="D60" s="63"/>
       <c r="E60" s="64"/>
-      <c r="F60" s="142"/>
+      <c r="F60" s="131"/>
       <c r="G60" s="65"/>
       <c r="H60" s="59"/>
       <c r="I60" s="2"/>
@@ -2482,7 +2582,7 @@
       <c r="C61" s="62"/>
       <c r="D61" s="63"/>
       <c r="E61" s="64"/>
-      <c r="F61" s="142"/>
+      <c r="F61" s="131"/>
       <c r="G61" s="65"/>
       <c r="H61" s="59"/>
       <c r="I61" s="2"/>
@@ -2493,7 +2593,7 @@
       <c r="C62" s="62"/>
       <c r="D62" s="63"/>
       <c r="E62" s="64"/>
-      <c r="F62" s="142"/>
+      <c r="F62" s="131"/>
       <c r="G62" s="65"/>
       <c r="H62" s="59"/>
       <c r="I62" s="2"/>
@@ -2504,7 +2604,7 @@
       <c r="C63" s="62"/>
       <c r="D63" s="63"/>
       <c r="E63" s="64"/>
-      <c r="F63" s="142"/>
+      <c r="F63" s="131"/>
       <c r="G63" s="65"/>
       <c r="H63" s="59"/>
       <c r="I63" s="2"/>
@@ -2515,7 +2615,7 @@
       <c r="C64" s="62"/>
       <c r="D64" s="63"/>
       <c r="E64" s="64"/>
-      <c r="F64" s="142"/>
+      <c r="F64" s="131"/>
       <c r="G64" s="65"/>
       <c r="H64" s="59"/>
       <c r="I64" s="2"/>
@@ -2526,7 +2626,7 @@
       <c r="C65" s="62"/>
       <c r="D65" s="63"/>
       <c r="E65" s="64"/>
-      <c r="F65" s="142"/>
+      <c r="F65" s="131"/>
       <c r="G65" s="65"/>
       <c r="H65" s="59"/>
       <c r="I65" s="2"/>
@@ -2537,7 +2637,7 @@
       <c r="C66" s="62"/>
       <c r="D66" s="63"/>
       <c r="E66" s="64"/>
-      <c r="F66" s="142"/>
+      <c r="F66" s="131"/>
       <c r="G66" s="65"/>
       <c r="H66" s="59"/>
     </row>
@@ -2547,7 +2647,7 @@
       <c r="C67" s="67"/>
       <c r="D67" s="68"/>
       <c r="E67" s="69"/>
-      <c r="F67" s="143"/>
+      <c r="F67" s="132"/>
       <c r="G67" s="70"/>
       <c r="H67" s="59"/>
     </row>
@@ -2579,25 +2679,25 @@
   <sheetData>
     <row r="9" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="4:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="121"/>
+      <c r="D10" s="120"/>
     </row>
     <row r="11" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D11" s="122"/>
+      <c r="D11" s="121"/>
     </row>
     <row r="12" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D12" s="122"/>
+      <c r="D12" s="121"/>
     </row>
     <row r="13" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D13" s="122"/>
+      <c r="D13" s="121"/>
     </row>
     <row r="14" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D14" s="122"/>
+      <c r="D14" s="121"/>
     </row>
     <row r="15" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D15" s="122"/>
+      <c r="D15" s="121"/>
     </row>
     <row r="16" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D16" s="123"/>
+      <c r="D16" s="122"/>
     </row>
     <row r="17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -2619,453 +2719,453 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" style="78" customWidth="1"/>
-    <col min="2" max="2" width="14" style="78" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="78"/>
+    <col min="1" max="1" width="3.42578125" style="77" customWidth="1"/>
+    <col min="2" max="2" width="14" style="77" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="77"/>
     <col min="4" max="4" width="20" style="50" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" style="78" customWidth="1"/>
-    <col min="6" max="6" width="5.28515625" style="83" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="77" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" style="82" customWidth="1"/>
     <col min="9" max="9" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:26" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="134" t="s">
+      <c r="B2" s="142" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="134"/>
-      <c r="D2" s="134"/>
-      <c r="E2" s="134"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134"/>
-      <c r="I2" s="134"/>
-      <c r="J2" s="134"/>
-      <c r="Z2" s="118" t="s">
+      <c r="C2" s="142"/>
+      <c r="D2" s="142"/>
+      <c r="E2" s="142"/>
+      <c r="F2" s="142"/>
+      <c r="G2" s="142"/>
+      <c r="H2" s="142"/>
+      <c r="I2" s="142"/>
+      <c r="J2" s="142"/>
+      <c r="Z2" s="117" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="2:26" ht="33.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="79" t="s">
+      <c r="B3" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="80" t="s">
+      <c r="C3" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="81" t="s">
+      <c r="D3" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="82" t="s">
+      <c r="E3" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="83"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
     </row>
     <row r="4" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B4" s="84"/>
-      <c r="C4" s="85"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="87">
+      <c r="B4" s="83"/>
+      <c r="C4" s="84"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="86">
         <f>D4</f>
         <v>0</v>
       </c>
-      <c r="F4" s="88"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="89"/>
-      <c r="I4" s="90"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="88"/>
+      <c r="I4" s="89"/>
       <c r="J4" s="20">
         <f>E47+I4</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B5" s="84"/>
-      <c r="C5" s="85"/>
-      <c r="D5" s="86"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="85"/>
       <c r="E5" s="20">
         <f>E4+D5</f>
         <v>0</v>
       </c>
-      <c r="G5" s="84"/>
-      <c r="H5" s="89"/>
-      <c r="I5" s="90"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="89"/>
       <c r="J5" s="20">
         <f>J4+I5</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B6" s="84"/>
-      <c r="C6" s="85"/>
-      <c r="D6" s="86"/>
+      <c r="B6" s="83"/>
+      <c r="C6" s="84"/>
+      <c r="D6" s="85"/>
       <c r="E6" s="20">
         <f t="shared" ref="E6:E47" si="0">E5+D6</f>
         <v>0</v>
       </c>
-      <c r="F6" s="91"/>
-      <c r="G6" s="84"/>
-      <c r="H6" s="89"/>
-      <c r="I6" s="90"/>
+      <c r="F6" s="90"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="88"/>
+      <c r="I6" s="89"/>
       <c r="J6" s="20">
         <f t="shared" ref="J6:J29" si="1">J5+I6</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B7" s="84"/>
-      <c r="C7" s="85"/>
-      <c r="D7" s="86"/>
+      <c r="B7" s="83"/>
+      <c r="C7" s="84"/>
+      <c r="D7" s="85"/>
       <c r="E7" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F7" s="91"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="89"/>
-      <c r="I7" s="90"/>
+      <c r="F7" s="90"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="88"/>
+      <c r="I7" s="89"/>
       <c r="J7" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B8" s="84"/>
-      <c r="C8" s="85"/>
-      <c r="D8" s="86"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="84"/>
+      <c r="D8" s="85"/>
       <c r="E8" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G8" s="84"/>
-      <c r="H8" s="89"/>
-      <c r="I8" s="90"/>
+      <c r="G8" s="83"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="89"/>
       <c r="J8" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B9" s="84"/>
-      <c r="C9" s="85"/>
-      <c r="D9" s="86"/>
+      <c r="B9" s="83"/>
+      <c r="C9" s="84"/>
+      <c r="D9" s="85"/>
       <c r="E9" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G9" s="84"/>
-      <c r="H9" s="92"/>
-      <c r="I9" s="86"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="91"/>
+      <c r="I9" s="85"/>
       <c r="J9" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B10" s="93"/>
-      <c r="C10" s="94"/>
+      <c r="B10" s="92"/>
+      <c r="C10" s="93"/>
       <c r="D10" s="21"/>
       <c r="E10" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G10" s="84"/>
-      <c r="H10" s="92"/>
-      <c r="I10" s="86"/>
+      <c r="G10" s="83"/>
+      <c r="H10" s="91"/>
+      <c r="I10" s="85"/>
       <c r="J10" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B11" s="93"/>
-      <c r="C11" s="94"/>
+      <c r="B11" s="92"/>
+      <c r="C11" s="93"/>
       <c r="D11" s="21"/>
       <c r="E11" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G11" s="84"/>
-      <c r="H11" s="92"/>
-      <c r="I11" s="86"/>
+      <c r="G11" s="83"/>
+      <c r="H11" s="91"/>
+      <c r="I11" s="85"/>
       <c r="J11" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B12" s="93"/>
-      <c r="C12" s="94"/>
+      <c r="B12" s="92"/>
+      <c r="C12" s="93"/>
       <c r="D12" s="21"/>
       <c r="E12" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G12" s="84"/>
-      <c r="H12" s="92"/>
-      <c r="I12" s="86"/>
+      <c r="G12" s="83"/>
+      <c r="H12" s="91"/>
+      <c r="I12" s="85"/>
       <c r="J12" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B13" s="93"/>
-      <c r="C13" s="94"/>
+      <c r="B13" s="92"/>
+      <c r="C13" s="93"/>
       <c r="D13" s="21"/>
       <c r="E13" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G13" s="84"/>
-      <c r="H13" s="92"/>
-      <c r="I13" s="86"/>
+      <c r="G13" s="83"/>
+      <c r="H13" s="91"/>
+      <c r="I13" s="85"/>
       <c r="J13" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B14" s="93"/>
-      <c r="C14" s="94"/>
+      <c r="B14" s="92"/>
+      <c r="C14" s="93"/>
       <c r="D14" s="21"/>
       <c r="E14" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G14" s="84"/>
-      <c r="H14" s="92"/>
-      <c r="I14" s="86"/>
+      <c r="G14" s="83"/>
+      <c r="H14" s="91"/>
+      <c r="I14" s="85"/>
       <c r="J14" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B15" s="93"/>
-      <c r="C15" s="94"/>
+      <c r="B15" s="92"/>
+      <c r="C15" s="93"/>
       <c r="D15" s="21"/>
       <c r="E15" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G15" s="84"/>
-      <c r="H15" s="92"/>
-      <c r="I15" s="86"/>
+      <c r="G15" s="83"/>
+      <c r="H15" s="91"/>
+      <c r="I15" s="85"/>
       <c r="J15" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B16" s="93"/>
-      <c r="C16" s="94"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="93"/>
       <c r="D16" s="21"/>
       <c r="E16" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G16" s="84"/>
-      <c r="H16" s="92"/>
-      <c r="I16" s="86"/>
+      <c r="G16" s="83"/>
+      <c r="H16" s="91"/>
+      <c r="I16" s="85"/>
       <c r="J16" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="93"/>
-      <c r="C17" s="94"/>
+      <c r="B17" s="92"/>
+      <c r="C17" s="93"/>
       <c r="D17" s="21"/>
       <c r="E17" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G17" s="84"/>
-      <c r="H17" s="89"/>
-      <c r="I17" s="86"/>
+      <c r="G17" s="83"/>
+      <c r="H17" s="88"/>
+      <c r="I17" s="85"/>
       <c r="J17" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="93"/>
-      <c r="C18" s="94"/>
+      <c r="B18" s="92"/>
+      <c r="C18" s="93"/>
       <c r="D18" s="21"/>
       <c r="E18" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G18" s="84"/>
-      <c r="H18" s="89"/>
-      <c r="I18" s="86"/>
+      <c r="G18" s="83"/>
+      <c r="H18" s="88"/>
+      <c r="I18" s="85"/>
       <c r="J18" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="93"/>
-      <c r="C19" s="94"/>
+      <c r="B19" s="92"/>
+      <c r="C19" s="93"/>
       <c r="D19" s="21"/>
       <c r="E19" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G19" s="84"/>
-      <c r="H19" s="89"/>
-      <c r="I19" s="86"/>
+      <c r="G19" s="83"/>
+      <c r="H19" s="88"/>
+      <c r="I19" s="85"/>
       <c r="J19" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="93"/>
-      <c r="C20" s="94"/>
+      <c r="B20" s="92"/>
+      <c r="C20" s="93"/>
       <c r="D20" s="21"/>
       <c r="E20" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G20" s="84"/>
-      <c r="H20" s="89"/>
-      <c r="I20" s="90"/>
+      <c r="G20" s="83"/>
+      <c r="H20" s="88"/>
+      <c r="I20" s="89"/>
       <c r="J20" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="93"/>
-      <c r="C21" s="94"/>
+      <c r="B21" s="92"/>
+      <c r="C21" s="93"/>
       <c r="D21" s="21"/>
       <c r="E21" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G21" s="84"/>
-      <c r="H21" s="89"/>
-      <c r="I21" s="90"/>
+      <c r="G21" s="83"/>
+      <c r="H21" s="88"/>
+      <c r="I21" s="89"/>
       <c r="J21" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="93"/>
-      <c r="C22" s="94"/>
+      <c r="B22" s="92"/>
+      <c r="C22" s="93"/>
       <c r="D22" s="21"/>
       <c r="E22" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G22" s="84"/>
-      <c r="H22" s="89"/>
-      <c r="I22" s="90"/>
+      <c r="G22" s="83"/>
+      <c r="H22" s="88"/>
+      <c r="I22" s="89"/>
       <c r="J22" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="93"/>
-      <c r="C23" s="94"/>
+      <c r="B23" s="92"/>
+      <c r="C23" s="93"/>
       <c r="D23" s="21"/>
       <c r="E23" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G23" s="84"/>
-      <c r="H23" s="89"/>
-      <c r="I23" s="90"/>
+      <c r="G23" s="83"/>
+      <c r="H23" s="88"/>
+      <c r="I23" s="89"/>
       <c r="J23" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="93"/>
-      <c r="C24" s="94"/>
+      <c r="B24" s="92"/>
+      <c r="C24" s="93"/>
       <c r="D24" s="21"/>
       <c r="E24" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G24" s="84"/>
-      <c r="H24" s="89"/>
-      <c r="I24" s="90"/>
+      <c r="G24" s="83"/>
+      <c r="H24" s="88"/>
+      <c r="I24" s="89"/>
       <c r="J24" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="93"/>
-      <c r="C25" s="94"/>
+      <c r="B25" s="92"/>
+      <c r="C25" s="93"/>
       <c r="D25" s="21"/>
       <c r="E25" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G25" s="84"/>
-      <c r="H25" s="89"/>
-      <c r="I25" s="95"/>
+      <c r="G25" s="83"/>
+      <c r="H25" s="88"/>
+      <c r="I25" s="94"/>
       <c r="J25" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="93"/>
-      <c r="C26" s="94"/>
+      <c r="B26" s="92"/>
+      <c r="C26" s="93"/>
       <c r="D26" s="21"/>
       <c r="E26" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G26" s="84"/>
-      <c r="H26" s="89"/>
-      <c r="I26" s="95"/>
+      <c r="G26" s="83"/>
+      <c r="H26" s="88"/>
+      <c r="I26" s="94"/>
       <c r="J26" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="93"/>
-      <c r="C27" s="94"/>
+      <c r="B27" s="92"/>
+      <c r="C27" s="93"/>
       <c r="D27" s="21"/>
       <c r="E27" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G27" s="96"/>
-      <c r="H27" s="97"/>
-      <c r="I27" s="98"/>
+      <c r="G27" s="95"/>
+      <c r="H27" s="96"/>
+      <c r="I27" s="97"/>
       <c r="J27" s="20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="93"/>
-      <c r="C28" s="94"/>
+      <c r="B28" s="92"/>
+      <c r="C28" s="93"/>
       <c r="D28" s="21"/>
       <c r="E28" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F28" s="99"/>
-      <c r="G28" s="100">
+      <c r="F28" s="98"/>
+      <c r="G28" s="99">
         <v>44965</v>
       </c>
-      <c r="H28" s="119" t="s">
+      <c r="H28" s="118" t="s">
         <v>16</v>
       </c>
-      <c r="I28" s="120">
+      <c r="I28" s="119">
         <v>-2029341.58</v>
       </c>
       <c r="J28" s="20">
@@ -3074,177 +3174,177 @@
       </c>
     </row>
     <row r="29" spans="2:10" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B29" s="93"/>
-      <c r="C29" s="94"/>
+      <c r="B29" s="92"/>
+      <c r="C29" s="93"/>
       <c r="D29" s="21"/>
       <c r="E29" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G29" s="101"/>
-      <c r="H29" s="101"/>
-      <c r="I29" s="101"/>
+      <c r="G29" s="100"/>
+      <c r="H29" s="100"/>
+      <c r="I29" s="100"/>
       <c r="J29" s="20">
         <f t="shared" si="1"/>
         <v>-2029341.58</v>
       </c>
     </row>
     <row r="30" spans="2:10" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B30" s="93"/>
-      <c r="C30" s="94"/>
+      <c r="B30" s="92"/>
+      <c r="C30" s="93"/>
       <c r="D30" s="21"/>
       <c r="E30" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G30" s="101"/>
-      <c r="H30" s="101"/>
-      <c r="I30" s="101"/>
-      <c r="J30" s="102"/>
+      <c r="G30" s="100"/>
+      <c r="H30" s="100"/>
+      <c r="I30" s="100"/>
+      <c r="J30" s="101"/>
     </row>
     <row r="31" spans="2:10" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B31" s="53"/>
-      <c r="C31" s="103"/>
-      <c r="D31" s="104"/>
+      <c r="C31" s="102"/>
+      <c r="D31" s="103"/>
       <c r="E31" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G31" s="101"/>
-      <c r="H31" s="101"/>
-      <c r="I31" s="101"/>
-      <c r="J31" s="102"/>
+      <c r="G31" s="100"/>
+      <c r="H31" s="100"/>
+      <c r="I31" s="100"/>
+      <c r="J31" s="101"/>
     </row>
     <row r="32" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B32" s="84"/>
-      <c r="C32" s="92"/>
-      <c r="D32" s="105"/>
+      <c r="B32" s="83"/>
+      <c r="C32" s="91"/>
+      <c r="D32" s="104"/>
       <c r="E32" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="B33" s="84"/>
-      <c r="C33" s="92"/>
-      <c r="D33" s="105"/>
+      <c r="B33" s="83"/>
+      <c r="C33" s="91"/>
+      <c r="D33" s="104"/>
       <c r="E33" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="B34" s="84"/>
-      <c r="C34" s="92"/>
-      <c r="D34" s="105"/>
+      <c r="B34" s="83"/>
+      <c r="C34" s="91"/>
+      <c r="D34" s="104"/>
       <c r="E34" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="84"/>
-      <c r="C35" s="92"/>
-      <c r="D35" s="86"/>
+      <c r="B35" s="83"/>
+      <c r="C35" s="91"/>
+      <c r="D35" s="85"/>
       <c r="E35" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="84"/>
-      <c r="C36" s="92"/>
-      <c r="D36" s="86"/>
+      <c r="B36" s="83"/>
+      <c r="C36" s="91"/>
+      <c r="D36" s="85"/>
       <c r="E36" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="84"/>
-      <c r="C37" s="92"/>
-      <c r="D37" s="86"/>
+      <c r="B37" s="83"/>
+      <c r="C37" s="91"/>
+      <c r="D37" s="85"/>
       <c r="E37" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="84"/>
-      <c r="C38" s="92"/>
-      <c r="D38" s="86"/>
+      <c r="B38" s="83"/>
+      <c r="C38" s="91"/>
+      <c r="D38" s="85"/>
       <c r="E38" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="84"/>
-      <c r="C39" s="92"/>
-      <c r="D39" s="86"/>
+      <c r="B39" s="83"/>
+      <c r="C39" s="91"/>
+      <c r="D39" s="85"/>
       <c r="E39" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="84"/>
-      <c r="C40" s="92"/>
-      <c r="D40" s="86"/>
+      <c r="B40" s="83"/>
+      <c r="C40" s="91"/>
+      <c r="D40" s="85"/>
       <c r="E40" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="84"/>
-      <c r="C41" s="92"/>
-      <c r="D41" s="86"/>
-      <c r="E41" s="106">
+      <c r="B41" s="83"/>
+      <c r="C41" s="91"/>
+      <c r="D41" s="85"/>
+      <c r="E41" s="105">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="84"/>
-      <c r="C42" s="92"/>
-      <c r="D42" s="86"/>
+      <c r="B42" s="83"/>
+      <c r="C42" s="91"/>
+      <c r="D42" s="85"/>
       <c r="E42" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="84"/>
-      <c r="C43" s="92"/>
-      <c r="D43" s="86"/>
+      <c r="B43" s="83"/>
+      <c r="C43" s="91"/>
+      <c r="D43" s="85"/>
       <c r="E43" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="84"/>
-      <c r="C44" s="92"/>
-      <c r="D44" s="86"/>
+      <c r="B44" s="83"/>
+      <c r="C44" s="91"/>
+      <c r="D44" s="85"/>
       <c r="E44" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="84"/>
-      <c r="C45" s="89"/>
-      <c r="D45" s="86"/>
+      <c r="B45" s="83"/>
+      <c r="C45" s="88"/>
+      <c r="D45" s="85"/>
       <c r="E45" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="84"/>
-      <c r="C46" s="89"/>
-      <c r="D46" s="86"/>
+      <c r="B46" s="83"/>
+      <c r="C46" s="88"/>
+      <c r="D46" s="85"/>
       <c r="E46" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3252,9 +3352,9 @@
       <c r="F46"/>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="84"/>
-      <c r="C47" s="89"/>
-      <c r="D47" s="86"/>
+      <c r="B47" s="83"/>
+      <c r="C47" s="88"/>
+      <c r="D47" s="85"/>
       <c r="E47" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3262,71 +3362,71 @@
       <c r="F47"/>
     </row>
     <row r="48" spans="2:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="C48" s="83"/>
+      <c r="C48" s="82"/>
       <c r="D48"/>
-      <c r="E48" s="107"/>
+      <c r="E48" s="106"/>
       <c r="F48"/>
     </row>
     <row r="49" spans="2:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="C49" s="83"/>
+      <c r="C49" s="82"/>
       <c r="D49"/>
-      <c r="E49" s="107"/>
+      <c r="E49" s="106"/>
       <c r="F49"/>
     </row>
     <row r="50" spans="2:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="C50" s="83"/>
+      <c r="C50" s="82"/>
       <c r="D50"/>
-      <c r="E50" s="107"/>
+      <c r="E50" s="106"/>
       <c r="F50"/>
     </row>
     <row r="51" spans="2:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="C51" s="83"/>
+      <c r="C51" s="82"/>
       <c r="D51"/>
-      <c r="E51" s="107"/>
+      <c r="E51" s="106"/>
       <c r="F51"/>
     </row>
     <row r="52" spans="2:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="C52" s="83"/>
+      <c r="C52" s="82"/>
       <c r="D52"/>
-      <c r="E52" s="107"/>
+      <c r="E52" s="106"/>
       <c r="F52"/>
     </row>
     <row r="53" spans="2:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="C53" s="83"/>
+      <c r="C53" s="82"/>
       <c r="D53"/>
-      <c r="E53" s="107"/>
+      <c r="E53" s="106"/>
       <c r="F53"/>
     </row>
     <row r="54" spans="2:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="C54" s="83"/>
-      <c r="D54" s="108" t="s">
+      <c r="C54" s="82"/>
+      <c r="D54" s="107" t="s">
         <v>17</v>
       </c>
       <c r="E54"/>
       <c r="F54"/>
     </row>
     <row r="55" spans="2:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="C55" s="83"/>
+      <c r="C55" s="82"/>
       <c r="D55"/>
       <c r="E55"/>
       <c r="F55"/>
     </row>
     <row r="56" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B56" s="109">
+      <c r="B56" s="108">
         <v>44892</v>
       </c>
-      <c r="C56" s="110" t="s">
+      <c r="C56" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="D56" s="111">
+      <c r="D56" s="110">
         <v>1884182.28</v>
       </c>
       <c r="E56"/>
       <c r="F56"/>
     </row>
     <row r="57" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B57" s="109"/>
-      <c r="C57" s="112" t="s">
+      <c r="B57" s="108"/>
+      <c r="C57" s="111" t="s">
         <v>18</v>
       </c>
       <c r="D57" s="21">
@@ -3336,24 +3436,24 @@
       <c r="F57"/>
     </row>
     <row r="58" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="109">
+      <c r="B58" s="108">
         <v>44924</v>
       </c>
-      <c r="C58" s="113" t="s">
+      <c r="C58" s="112" t="s">
         <v>19</v>
       </c>
-      <c r="D58" s="114">
+      <c r="D58" s="113">
         <v>-184075.5</v>
       </c>
       <c r="E58"/>
       <c r="F58"/>
     </row>
     <row r="59" spans="2:6" ht="20.25" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="109"/>
-      <c r="C59" s="115" t="s">
+      <c r="B59" s="108"/>
+      <c r="C59" s="114" t="s">
         <v>20</v>
       </c>
-      <c r="D59" s="116">
+      <c r="D59" s="115">
         <f>SUM(D56:D58)</f>
         <v>1008356.78</v>
       </c>
@@ -3361,15 +3461,15 @@
       <c r="F59"/>
     </row>
     <row r="60" spans="2:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="B60" s="117"/>
-      <c r="C60" s="83"/>
+      <c r="B60" s="116"/>
+      <c r="C60" s="82"/>
       <c r="D60"/>
       <c r="E60"/>
       <c r="F60"/>
     </row>
     <row r="61" spans="2:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="B61" s="117"/>
-      <c r="C61" s="83"/>
+      <c r="B61" s="116"/>
+      <c r="C61" s="82"/>
       <c r="D61"/>
       <c r="E61"/>
       <c r="F61"/>

</xml_diff>